<commit_message>
Physical Edit Distance modified, show distance and freqeuncy with corrected word
</commit_message>
<xml_diff>
--- a/documents/cheonjiin_physical_distance.xlsx
+++ b/documents/cheonjiin_physical_distance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\중앙대학교\3학년 1학기\오픈소스SW프로젝트\과제\Term Project\ChinJiIn\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CD72E83-F6FC-4654-8F40-EA52B41DACCC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F57409C7-565E-45BB-82EB-AF9BE38F18F4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
   <si>
     <t>ㅣ</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -128,6 +128,10 @@
   </si>
   <si>
     <t>거리 평균</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>같은 글자에 대한 거리</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -178,7 +182,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -251,37 +255,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -301,6 +279,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -310,16 +294,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -605,7 +580,7 @@
   <dimension ref="B2:R13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+      <selection activeCell="V15" sqref="V15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -617,7 +592,7 @@
       <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="7" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="2" t="s">
@@ -657,8 +632,8 @@
       <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="1">
-        <v>0</v>
+      <c r="C3" s="6">
+        <v>0.5</v>
       </c>
       <c r="D3" s="1">
         <v>1</v>
@@ -695,14 +670,14 @@
       <c r="R3" s="3"/>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.4">
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
       </c>
-      <c r="D4" s="1">
-        <v>0</v>
+      <c r="D4" s="6">
+        <v>0.5</v>
       </c>
       <c r="E4" s="1">
         <v>1</v>
@@ -732,12 +707,12 @@
         <v>2</v>
       </c>
       <c r="N4" s="3"/>
-      <c r="O4" s="10" t="s">
+      <c r="O4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="P4" s="11">
+      <c r="P4" s="1">
         <f>AVERAGE(C3:C13, D4:D13, E5:E13, F6:F13, G7:G13, H8:H13, I9:I13, J10:J13, K11:K13, L12:L13, M13:M13)</f>
-        <v>1.5668181818181812</v>
+        <v>1.6501515151515145</v>
       </c>
       <c r="Q4" s="3"/>
       <c r="R4" s="3"/>
@@ -752,8 +727,8 @@
       <c r="D5" s="1">
         <v>1</v>
       </c>
-      <c r="E5" s="1">
-        <v>0</v>
+      <c r="E5" s="6">
+        <v>0.5</v>
       </c>
       <c r="F5" s="1">
         <v>2.23</v>
@@ -780,10 +755,14 @@
         <v>1</v>
       </c>
       <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="3"/>
-      <c r="R5" s="3"/>
+      <c r="O5" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="12"/>
+      <c r="R5" s="1">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B6" s="4" t="s">
@@ -798,8 +777,8 @@
       <c r="E6" s="1">
         <v>2.23</v>
       </c>
-      <c r="F6" s="1">
-        <v>0</v>
+      <c r="F6" s="6">
+        <v>0.5</v>
       </c>
       <c r="G6" s="1">
         <v>1</v>
@@ -844,8 +823,8 @@
       <c r="F7" s="1">
         <v>1</v>
       </c>
-      <c r="G7" s="1">
-        <v>0</v>
+      <c r="G7" s="6">
+        <v>0.5</v>
       </c>
       <c r="H7" s="1">
         <v>1</v>
@@ -890,8 +869,8 @@
       <c r="G8" s="1">
         <v>1</v>
       </c>
-      <c r="H8" s="1">
-        <v>0</v>
+      <c r="H8" s="6">
+        <v>0.5</v>
       </c>
       <c r="I8" s="1">
         <v>2.23</v>
@@ -909,12 +888,12 @@
         <v>1.41</v>
       </c>
       <c r="N8" s="3"/>
-      <c r="O8" s="7" t="s">
+      <c r="O8" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="8"/>
-      <c r="R8" s="9"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="11"/>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B9" s="4" t="s">
@@ -938,8 +917,8 @@
       <c r="H9" s="1">
         <v>2.23</v>
       </c>
-      <c r="I9" s="1">
-        <v>0</v>
+      <c r="I9" s="6">
+        <v>0.5</v>
       </c>
       <c r="J9" s="1">
         <v>1</v>
@@ -992,8 +971,8 @@
       <c r="I10" s="1">
         <v>1</v>
       </c>
-      <c r="J10" s="1">
-        <v>0</v>
+      <c r="J10" s="6">
+        <v>0.5</v>
       </c>
       <c r="K10" s="1">
         <v>1</v>
@@ -1044,8 +1023,8 @@
       <c r="J11" s="1">
         <v>1</v>
       </c>
-      <c r="K11" s="1">
-        <v>0</v>
+      <c r="K11" s="6">
+        <v>0.5</v>
       </c>
       <c r="L11" s="1">
         <v>1.41</v>
@@ -1096,8 +1075,8 @@
       <c r="K12" s="1">
         <v>1.41</v>
       </c>
-      <c r="L12" s="1">
-        <v>0</v>
+      <c r="L12" s="6">
+        <v>0.5</v>
       </c>
       <c r="M12" s="1">
         <v>3.6</v>
@@ -1145,7 +1124,7 @@
         <v>3.6</v>
       </c>
       <c r="M13" s="6">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
@@ -1154,8 +1133,9 @@
       <c r="R13" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="O8:R8"/>
+    <mergeCell ref="O5:Q5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
physical distace about whitespace re-calcuated
</commit_message>
<xml_diff>
--- a/documents/cheonjiin_physical_distance.xlsx
+++ b/documents/cheonjiin_physical_distance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\중앙대학교\3학년 1학기\오픈소스SW프로젝트\과제\Term Project\ChinJiIn\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F57409C7-565E-45BB-82EB-AF9BE38F18F4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{301D8124-FB26-4D05-AE6D-A2600EF9A21E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -259,7 +259,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -283,6 +283,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -577,10 +580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:R13"/>
+  <dimension ref="B2:R17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V15" sqref="V15"/>
+      <selection activeCell="L19" sqref="K19:L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -663,7 +666,7 @@
         <v>3.16</v>
       </c>
       <c r="M3" s="1">
-        <v>3</v>
+        <v>3.6</v>
       </c>
       <c r="N3" s="3"/>
       <c r="Q3" s="3"/>
@@ -704,7 +707,7 @@
         <v>3</v>
       </c>
       <c r="M4" s="1">
-        <v>2</v>
+        <v>3.16</v>
       </c>
       <c r="N4" s="3"/>
       <c r="O4" s="1" t="s">
@@ -712,7 +715,7 @@
       </c>
       <c r="P4" s="1">
         <f>AVERAGE(C3:C13, D4:D13, E5:E13, F6:F13, G7:G13, H8:H13, I9:I13, J10:J13, K11:K13, L12:L13, M13:M13)</f>
-        <v>1.6501515151515145</v>
+        <v>1.6107575757575756</v>
       </c>
       <c r="Q4" s="3"/>
       <c r="R4" s="3"/>
@@ -752,14 +755,14 @@
         <v>3.16</v>
       </c>
       <c r="M5" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N5" s="3"/>
-      <c r="O5" s="12" t="s">
+      <c r="O5" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="P5" s="12"/>
-      <c r="Q5" s="12"/>
+      <c r="P5" s="13"/>
+      <c r="Q5" s="13"/>
       <c r="R5" s="1">
         <v>0.5</v>
       </c>
@@ -799,7 +802,7 @@
         <v>2.23</v>
       </c>
       <c r="M6" s="1">
-        <v>3.16</v>
+        <v>2.82</v>
       </c>
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
@@ -885,15 +888,15 @@
         <v>2.23</v>
       </c>
       <c r="M8" s="1">
-        <v>1.41</v>
+        <v>2</v>
       </c>
       <c r="N8" s="3"/>
-      <c r="O8" s="9" t="s">
+      <c r="O8" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="P8" s="10"/>
-      <c r="Q8" s="10"/>
-      <c r="R8" s="11"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11"/>
+      <c r="R8" s="12"/>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B9" s="4" t="s">
@@ -930,7 +933,7 @@
         <v>1.41</v>
       </c>
       <c r="M9" s="1">
-        <v>3.6</v>
+        <v>2.23</v>
       </c>
       <c r="N9" s="3"/>
       <c r="O9" s="5" t="s">
@@ -942,9 +945,6 @@
       <c r="Q9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="R9" s="5" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B10" s="4" t="s">
@@ -981,7 +981,7 @@
         <v>1</v>
       </c>
       <c r="M10" s="1">
-        <v>2.82</v>
+        <v>1.41</v>
       </c>
       <c r="N10" s="3"/>
       <c r="O10" s="1" t="s">
@@ -1030,7 +1030,7 @@
         <v>1.41</v>
       </c>
       <c r="M11" s="1">
-        <v>2.23</v>
+        <v>1</v>
       </c>
       <c r="N11" s="3"/>
       <c r="O11" s="1" t="s">
@@ -1079,49 +1079,50 @@
         <v>0.5</v>
       </c>
       <c r="M12" s="1">
-        <v>3.6</v>
+        <v>1</v>
       </c>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
       <c r="P12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="Q12" s="3"/>
-      <c r="R12" s="3"/>
+      <c r="Q12" s="9" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B13" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="D13" s="1">
+        <v>3.16</v>
+      </c>
+      <c r="E13" s="1">
         <v>3</v>
       </c>
-      <c r="D13" s="1">
-        <v>2</v>
-      </c>
-      <c r="E13" s="1">
-        <v>1</v>
-      </c>
       <c r="F13" s="1">
-        <v>3.16</v>
+        <v>2.82</v>
       </c>
       <c r="G13" s="1">
         <v>2.23</v>
       </c>
       <c r="H13" s="1">
-        <v>1.41</v>
+        <v>2</v>
       </c>
       <c r="I13" s="1">
-        <v>3.6</v>
+        <v>2.23</v>
       </c>
       <c r="J13" s="1">
-        <v>2.82</v>
+        <v>1.41</v>
       </c>
       <c r="K13" s="1">
-        <v>2.23</v>
+        <v>1</v>
       </c>
       <c r="L13" s="1">
-        <v>3.6</v>
+        <v>1</v>
       </c>
       <c r="M13" s="6">
         <v>0.5</v>
@@ -1131,6 +1132,47 @@
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
       <c r="R13" s="3"/>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.4">
+      <c r="O14">
+        <v>3.6</v>
+      </c>
+      <c r="P14">
+        <v>3.16</v>
+      </c>
+      <c r="Q14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.4">
+      <c r="O15">
+        <v>2.82</v>
+      </c>
+      <c r="P15">
+        <v>2.23</v>
+      </c>
+      <c r="Q15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.4">
+      <c r="O16">
+        <v>2.23</v>
+      </c>
+      <c r="P16">
+        <v>1.41</v>
+      </c>
+      <c r="Q16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="16:17" x14ac:dyDescent="0.4">
+      <c r="P17">
+        <v>1</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
non-cheonjiin input corruption hot-fix: fixed just not to make error, there's no weight in calculating distance
</commit_message>
<xml_diff>
--- a/documents/cheonjiin_physical_distance.xlsx
+++ b/documents/cheonjiin_physical_distance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\중앙대학교\3학년 1학기\오픈소스SW프로젝트\과제\Term Project\ChinJiIn\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{301D8124-FB26-4D05-AE6D-A2600EF9A21E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADA021AB-234C-43C5-AA82-23C4A5F7F244}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
   <si>
     <t>ㅣ</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -132,6 +132,10 @@
   </si>
   <si>
     <t>같은 글자에 대한 거리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ELSE</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -182,7 +186,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -255,11 +259,61 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -297,7 +351,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -580,15 +649,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:R17"/>
+  <dimension ref="B2:T14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L19" sqref="K19:L19"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:20" x14ac:dyDescent="0.4">
       <c r="B2" s="1" t="s">
         <v>22</v>
       </c>
@@ -625,13 +694,15 @@
       <c r="M2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="3"/>
+      <c r="N2" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
       <c r="R2" s="3"/>
     </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:20" x14ac:dyDescent="0.4">
       <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
@@ -668,11 +739,13 @@
       <c r="M3" s="1">
         <v>3.6</v>
       </c>
-      <c r="N3" s="3"/>
+      <c r="N3" s="9">
+        <v>1</v>
+      </c>
       <c r="Q3" s="3"/>
       <c r="R3" s="3"/>
     </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:20" x14ac:dyDescent="0.4">
       <c r="B4" s="8" t="s">
         <v>20</v>
       </c>
@@ -709,18 +782,20 @@
       <c r="M4" s="1">
         <v>3.16</v>
       </c>
-      <c r="N4" s="3"/>
-      <c r="O4" s="1" t="s">
+      <c r="N4" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="P4" s="1">
+      <c r="R4" s="9">
         <f>AVERAGE(C3:C13, D4:D13, E5:E13, F6:F13, G7:G13, H8:H13, I9:I13, J10:J13, K11:K13, L12:L13, M13:M13)</f>
         <v>1.6107575757575756</v>
       </c>
-      <c r="Q4" s="3"/>
-      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:20" x14ac:dyDescent="0.4">
       <c r="B5" s="4" t="s">
         <v>1</v>
       </c>
@@ -757,17 +832,19 @@
       <c r="M5" s="1">
         <v>3</v>
       </c>
-      <c r="N5" s="3"/>
-      <c r="O5" s="13" t="s">
+      <c r="N5" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="P5" s="13"/>
-      <c r="Q5" s="13"/>
-      <c r="R5" s="1">
+      <c r="R5" s="15"/>
+      <c r="S5" s="14"/>
+      <c r="T5" s="9">
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:20" x14ac:dyDescent="0.4">
       <c r="B6" s="4" t="s">
         <v>2</v>
       </c>
@@ -804,13 +881,15 @@
       <c r="M6" s="1">
         <v>2.82</v>
       </c>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
+      <c r="N6" s="9">
+        <v>1</v>
+      </c>
       <c r="Q6" s="3"/>
       <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
     </row>
-    <row r="7" spans="2:18" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:20" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B7" s="4" t="s">
         <v>3</v>
       </c>
@@ -847,13 +926,15 @@
       <c r="M7" s="1">
         <v>2.23</v>
       </c>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
+      <c r="N7" s="9">
+        <v>1</v>
+      </c>
       <c r="Q7" s="3"/>
       <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
     </row>
-    <row r="8" spans="2:18" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:20" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B8" s="4" t="s">
         <v>4</v>
       </c>
@@ -890,15 +971,17 @@
       <c r="M8" s="1">
         <v>2</v>
       </c>
-      <c r="N8" s="3"/>
-      <c r="O8" s="10" t="s">
+      <c r="N8" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="P8" s="11"/>
-      <c r="Q8" s="11"/>
-      <c r="R8" s="12"/>
+      <c r="R8" s="11"/>
+      <c r="S8" s="11"/>
+      <c r="T8" s="12"/>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:20" x14ac:dyDescent="0.4">
       <c r="B9" s="4" t="s">
         <v>5</v>
       </c>
@@ -935,18 +1018,20 @@
       <c r="M9" s="1">
         <v>2.23</v>
       </c>
-      <c r="N9" s="3"/>
-      <c r="O9" s="5" t="s">
+      <c r="N9" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="P9" s="5" t="s">
+      <c r="R9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="Q9" s="5" t="s">
+      <c r="S9" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:20" x14ac:dyDescent="0.4">
       <c r="B10" s="4" t="s">
         <v>6</v>
       </c>
@@ -983,19 +1068,21 @@
       <c r="M10" s="1">
         <v>1.41</v>
       </c>
-      <c r="N10" s="3"/>
-      <c r="O10" s="1" t="s">
+      <c r="N10" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="P10" s="1" t="s">
+      <c r="R10" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="Q10" s="1" t="s">
+      <c r="S10" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="R10" s="3"/>
+      <c r="T10" s="3"/>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:20" x14ac:dyDescent="0.4">
       <c r="B11" s="4" t="s">
         <v>7</v>
       </c>
@@ -1032,19 +1119,21 @@
       <c r="M11" s="1">
         <v>1</v>
       </c>
-      <c r="N11" s="3"/>
-      <c r="O11" s="1" t="s">
+      <c r="N11" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="P11" s="1" t="s">
+      <c r="R11" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="Q11" s="1" t="s">
+      <c r="S11" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="R11" s="3"/>
+      <c r="T11" s="3"/>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:20" x14ac:dyDescent="0.4">
       <c r="B12" s="4" t="s">
         <v>8</v>
       </c>
@@ -1081,103 +1170,107 @@
       <c r="M12" s="1">
         <v>1</v>
       </c>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="1" t="s">
+      <c r="N12" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="Q12" s="9" t="s">
+      <c r="S12" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.4">
-      <c r="B13" s="4" t="s">
+    <row r="13" spans="2:20" x14ac:dyDescent="0.4">
+      <c r="B13" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="17">
         <v>3.6</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="17">
         <v>3.16</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="17">
         <v>3</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13" s="17">
         <v>2.82</v>
       </c>
-      <c r="G13" s="1">
-        <v>2.23</v>
-      </c>
-      <c r="H13" s="1">
-        <v>2</v>
-      </c>
-      <c r="I13" s="1">
-        <v>2.23</v>
-      </c>
-      <c r="J13" s="1">
-        <v>1.41</v>
-      </c>
-      <c r="K13" s="1">
-        <v>1</v>
-      </c>
-      <c r="L13" s="1">
-        <v>1</v>
-      </c>
-      <c r="M13" s="6">
+      <c r="G13" s="17">
+        <v>2.23</v>
+      </c>
+      <c r="H13" s="17">
+        <v>2</v>
+      </c>
+      <c r="I13" s="17">
+        <v>2.23</v>
+      </c>
+      <c r="J13" s="17">
+        <v>1.41</v>
+      </c>
+      <c r="K13" s="17">
+        <v>1</v>
+      </c>
+      <c r="L13" s="17">
+        <v>1</v>
+      </c>
+      <c r="M13" s="18">
         <v>0.5</v>
       </c>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
+      <c r="N13" s="9">
+        <v>1</v>
+      </c>
       <c r="Q13" s="3"/>
       <c r="R13" s="3"/>
+      <c r="S13" s="3"/>
+      <c r="T13" s="3"/>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.4">
-      <c r="O14">
-        <v>3.6</v>
-      </c>
-      <c r="P14">
-        <v>3.16</v>
-      </c>
-      <c r="Q14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.4">
-      <c r="O15">
-        <v>2.82</v>
-      </c>
-      <c r="P15">
-        <v>2.23</v>
-      </c>
-      <c r="Q15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.4">
-      <c r="O16">
-        <v>2.23</v>
-      </c>
-      <c r="P16">
-        <v>1.41</v>
-      </c>
-      <c r="Q16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="16:17" x14ac:dyDescent="0.4">
-      <c r="P17">
-        <v>1</v>
-      </c>
-      <c r="Q17">
-        <v>0</v>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.4">
+      <c r="B14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="6">
+        <v>1</v>
+      </c>
+      <c r="D14" s="6">
+        <v>1</v>
+      </c>
+      <c r="E14" s="6">
+        <v>1</v>
+      </c>
+      <c r="F14" s="6">
+        <v>1</v>
+      </c>
+      <c r="G14" s="6">
+        <v>1</v>
+      </c>
+      <c r="H14" s="6">
+        <v>1</v>
+      </c>
+      <c r="I14" s="6">
+        <v>1</v>
+      </c>
+      <c r="J14" s="6">
+        <v>1</v>
+      </c>
+      <c r="K14" s="6">
+        <v>1</v>
+      </c>
+      <c r="L14" s="6">
+        <v>1</v>
+      </c>
+      <c r="M14" s="6">
+        <v>1</v>
+      </c>
+      <c r="N14" s="9">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="O8:R8"/>
-    <mergeCell ref="O5:Q5"/>
+    <mergeCell ref="Q5:S5"/>
+    <mergeCell ref="Q8:T8"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>